<commit_message>
Verlust Vogesen und Trikot Set Geld Hape eingetragen
</commit_message>
<xml_diff>
--- a/Dokumente/Ausstände CA.xlsx
+++ b/Dokumente/Ausstände CA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/LuGol/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/T3-Extern/SourceTree/cycling-adventures.org/Dokumente/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
   <si>
     <t>Ausstände CA</t>
   </si>
@@ -63,14 +63,21 @@
   </si>
   <si>
     <t>Marketing, Recht, Gründung, Kauf und Verkauf eines Reisebüros</t>
+  </si>
+  <si>
+    <t>Verlust Vogesen</t>
+  </si>
+  <si>
+    <t>Trikot Set Hape Bar eingesackt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-407]_-;\-* #,##0.00\ [$€-407]_-;_-* &quot;-&quot;??\ [$€-407]_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-407];[Red]\-#,##0.00\ [$€-407]"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -113,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -121,6 +128,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
@@ -417,7 +426,7 @@
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <f>Lutz!E2+Lukas!E2+Roli!E2</f>
-        <v>1084</v>
+        <v>699.85</v>
       </c>
     </row>
   </sheetData>
@@ -427,17 +436,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="14.5" style="8" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -447,7 +456,7 @@
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="4" t="s">
@@ -455,29 +464,29 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>4</v>
+      <c r="A2" s="6">
+        <v>42614</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" s="3">
-        <v>735</v>
+        <v>10</v>
+      </c>
+      <c r="C2" s="8">
+        <v>138</v>
       </c>
       <c r="E2" s="3">
         <f>SUM(C:C)</f>
-        <v>1084</v>
+        <v>699.85</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>4</v>
+      <c r="A3" s="5">
+        <v>42707</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="3">
-        <v>140</v>
+        <v>9</v>
+      </c>
+      <c r="C3" s="8">
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -487,30 +496,52 @@
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3">
+      <c r="C4" s="8">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="5">
-        <v>42707</v>
+      <c r="A5" t="s">
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="3">
-        <v>60</v>
+        <v>6</v>
+      </c>
+      <c r="C5" s="8">
+        <v>140</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="6">
-        <v>42614</v>
+      <c r="A6" t="s">
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="3">
-        <v>138</v>
+        <v>5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="6">
+        <v>42856</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="8">
+        <v>-284.14999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="6">
+        <v>42856</v>
+      </c>
+      <c r="B8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8">
+        <v>-100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>